<commit_message>
Solicitud gráfica guion 3 REC190
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion03/SolicitudGrafica_LE_08_03_REC190.xlsx
+++ b/fuentes/contenidos/grado08/guion03/SolicitudGrafica_LE_08_03_REC190.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19785" windowHeight="7650" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -22,11 +22,16 @@
     <definedName name="Ubicación">'Solicitud gráfica'!$M$2:$M$6</definedName>
   </definedNames>
   <calcPr calcId="152511" iterateCount="2" iterateDelta="10" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="207">
   <si>
     <t>Fecha:</t>
   </si>
@@ -590,13 +595,61 @@
     <t>Trabajar un video</t>
   </si>
   <si>
+    <t>Luz Amparo Rubiano</t>
+  </si>
+  <si>
+    <t>SHUTTER: 272128427</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHUTTER: 78719365 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHUTTER: 287779580 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHUTTER: 279796130 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHUTER: 208789036 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHUTTER: 45754267 </t>
+  </si>
+  <si>
+    <t>Fotografía</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Acción</t>
+  </si>
+  <si>
+    <t>Zapatos</t>
+  </si>
+  <si>
+    <t>Cráter</t>
+  </si>
+  <si>
+    <t>Célula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHUTTER: 212435689 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHUTTER: 222668197 </t>
+  </si>
+  <si>
+    <t>Osezno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHUTTER: 250892782 </t>
+  </si>
+  <si>
+    <t>Martillazo</t>
+  </si>
+  <si>
     <t>El texto prescriptivo</t>
-  </si>
-  <si>
-    <t>Luz Amparo Rubiano</t>
-  </si>
-  <si>
-    <t>Fotografía</t>
   </si>
   <si>
     <t>LE_08_03_REC190</t>
@@ -1022,11 +1075,11 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1035,7 +1088,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1043,17 +1096,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -1063,7 +1116,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1071,12 +1124,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1085,18 +1138,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1126,11 +1179,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1140,10 +1193,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1153,7 +1206,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
@@ -1227,16 +1280,16 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1244,23 +1297,23 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1762,157 +1815,20 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>559593</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>119063</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1572093</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>839063</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="1 Imagen"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12644437" y="2274094"/>
-          <a:ext cx="1012500" cy="720000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>607220</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>107157</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1530297</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>827157</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="3 Imagen"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12692064" y="3167063"/>
-          <a:ext cx="923077" cy="720000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>535782</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>59531</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1551456</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>779531</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="4 Imagen"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12620626" y="3952875"/>
-          <a:ext cx="1015674" cy="720000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>1038225</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1959,15 +1875,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1047750</xdr:colOff>
+          <xdr:colOff>1057275</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>866775</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2014,15 +1930,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2130,7 +2046,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>828675</xdr:colOff>
+          <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
@@ -2179,7 +2095,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>485775</xdr:rowOff>
         </xdr:from>
@@ -2234,7 +2150,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>485775</xdr:rowOff>
         </xdr:from>
@@ -2612,22 +2528,23 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.75" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.25" style="2" customWidth="1"/>
-    <col min="6" max="7" width="20.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="28.625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="29.75" style="15" customWidth="1"/>
+    <col min="10" max="10" width="34.875" style="15" customWidth="1"/>
     <col min="11" max="11" width="29.625" style="15" customWidth="1"/>
     <col min="12" max="12" width="20.375" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" hidden="1" customWidth="1"/>
@@ -2695,7 +2612,7 @@
       </c>
       <c r="D3" s="88"/>
       <c r="F3" s="80">
-        <v>42329</v>
+        <v>42341</v>
       </c>
       <c r="G3" s="81"/>
       <c r="H3" s="58"/>
@@ -2722,7 +2639,7 @@
         <v>54</v>
       </c>
       <c r="C4" s="87" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="D4" s="88"/>
       <c r="E4" s="5"/>
@@ -2754,7 +2671,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D5" s="90"/>
       <c r="E5" s="5"/>
@@ -2811,7 +2728,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>39</v>
@@ -2901,26 +2818,26 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
-      <c r="B10" s="62">
-        <v>199446704</v>
+      <c r="B10" s="62" t="s">
+        <v>188</v>
       </c>
       <c r="C10" s="20" t="str">
         <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso F6</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E10" s="63" t="s">
         <v>150</v>
       </c>
       <c r="F10" s="13" t="str">
-        <f t="shared" ref="F10" ca="1" si="1">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f ca="1">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>LE_08_03_REC190_IMG01.jpg</v>
       </c>
       <c r="G10" s="13" t="str">
@@ -2928,40 +2845,42 @@
         <v>350 x 230 px</v>
       </c>
       <c r="H10" s="13" t="str">
-        <f t="shared" ref="H10" ca="1" si="2">IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f ca="1">IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I10" s="13" t="str">
         <f ca="1">IF(OR($B10&lt;&gt;"",$J10&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v/>
       </c>
-      <c r="J10" s="63"/>
+      <c r="J10" s="63" t="s">
+        <v>195</v>
+      </c>
       <c r="K10" s="64"/>
       <c r="O10" s="2" t="str">
         <f>'Definición técnica de imagenes'!A12</f>
         <v>M12D</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="11" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="str">
-        <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
+        <f t="shared" ref="A11:A18" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="62">
-        <v>246570298</v>
+      <c r="B11" s="62" t="s">
+        <v>189</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F6</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E11" s="63" t="s">
         <v>150</v>
       </c>
       <c r="F11" s="13" t="str">
-        <f t="shared" ref="F11:F74" ca="1" si="4">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" ref="F11:F74" ca="1" si="2">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>LE_08_03_REC190_IMG02.jpg</v>
       </c>
       <c r="G11" s="13" t="str">
@@ -2969,40 +2888,42 @@
         <v>350 x 230 px</v>
       </c>
       <c r="H11" s="13" t="str">
-        <f t="shared" ref="H11:H74" ca="1" si="5">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" ref="H11:H74" ca="1" si="3">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I11" s="13" t="str">
         <f ca="1">IF(OR($B11&lt;&gt;"",$J11&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v/>
       </c>
-      <c r="J11" s="64"/>
+      <c r="J11" s="64" t="s">
+        <v>196</v>
+      </c>
       <c r="K11" s="65"/>
       <c r="O11" s="2" t="str">
         <f>'Definición técnica de imagenes'!A13</f>
         <v>M101</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>IMG03</v>
       </c>
-      <c r="B12" s="62">
-        <v>262868714</v>
+      <c r="B12" s="62" t="s">
+        <v>190</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F6</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E12" s="63" t="s">
         <v>150</v>
       </c>
       <c r="F12" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="2"/>
         <v>LE_08_03_REC190_IMG03.jpg</v>
       </c>
       <c r="G12" s="13" t="str">
@@ -3010,14 +2931,16 @@
         <v>350 x 230 px</v>
       </c>
       <c r="H12" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I12" s="13" t="str">
         <f ca="1">IF(OR($B12&lt;&gt;"",$J12&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v/>
       </c>
-      <c r="J12" s="64"/>
+      <c r="J12" s="64" t="s">
+        <v>197</v>
+      </c>
       <c r="K12" s="64"/>
       <c r="O12" s="2" t="str">
         <f>'Definición técnica de imagenes'!A18</f>
@@ -3026,33 +2949,41 @@
     </row>
     <row r="13" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B13" s="62"/>
+        <f t="shared" si="1"/>
+        <v>IMG04</v>
+      </c>
+      <c r="B13" s="62" t="s">
+        <v>191</v>
+      </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
+        <v>Recurso F6</v>
+      </c>
+      <c r="D13" s="63" t="s">
+        <v>194</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>155</v>
+      </c>
       <c r="F13" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="2"/>
+        <v>LE_08_03_REC190_IMG04n.jpg</v>
       </c>
       <c r="G13" s="13" t="str">
         <f ca="1">IF($F13&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>320 x 480 px</v>
       </c>
       <c r="H13" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
+        <f t="shared" ca="1" si="3"/>
+        <v>LE_08_03_REC190_IMG04a.jpg</v>
       </c>
       <c r="I13" s="13" t="str">
         <f ca="1">IF(OR($B13&lt;&gt;"",$J13&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v/>
-      </c>
-      <c r="J13" s="64"/>
+        <v>800 x 458 px</v>
+      </c>
+      <c r="J13" s="64" t="s">
+        <v>195</v>
+      </c>
       <c r="K13" s="64"/>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
@@ -3061,33 +2992,41 @@
     </row>
     <row r="14" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B14" s="62"/>
+        <f t="shared" si="1"/>
+        <v>IMG05</v>
+      </c>
+      <c r="B14" s="62" t="s">
+        <v>192</v>
+      </c>
       <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
+        <v>Recurso F6</v>
+      </c>
+      <c r="D14" s="63" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" s="63" t="s">
+        <v>155</v>
+      </c>
       <c r="F14" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="2"/>
+        <v>LE_08_03_REC190_IMG05n.jpg</v>
       </c>
       <c r="G14" s="13" t="str">
         <f ca="1">IF($F14&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>320 x 480 px</v>
       </c>
       <c r="H14" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
+        <f t="shared" ca="1" si="3"/>
+        <v>LE_08_03_REC190_IMG05a.jpg</v>
       </c>
       <c r="I14" s="13" t="str">
         <f ca="1">IF(OR($B14&lt;&gt;"",$J14&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v/>
-      </c>
-      <c r="J14" s="64"/>
+        <v>800 x 458 px</v>
+      </c>
+      <c r="J14" s="64" t="s">
+        <v>198</v>
+      </c>
       <c r="K14" s="64"/>
       <c r="O14" s="2" t="str">
         <f>'Definición técnica de imagenes'!A22</f>
@@ -3096,33 +3035,41 @@
     </row>
     <row r="15" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B15" s="62"/>
+        <f t="shared" si="1"/>
+        <v>IMG06</v>
+      </c>
+      <c r="B15" s="62" t="s">
+        <v>193</v>
+      </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
+        <v>Recurso F6</v>
+      </c>
+      <c r="D15" s="63" t="s">
+        <v>194</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>155</v>
+      </c>
       <c r="F15" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="2"/>
+        <v>LE_08_03_REC190_IMG06n.jpg</v>
       </c>
       <c r="G15" s="13" t="str">
         <f ca="1">IF($F15&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>320 x 480 px</v>
       </c>
       <c r="H15" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
+        <f t="shared" ca="1" si="3"/>
+        <v>LE_08_03_REC190_IMG06a.jpg</v>
       </c>
       <c r="I15" s="13" t="str">
         <f ca="1">IF(OR($B15&lt;&gt;"",$J15&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v/>
-      </c>
-      <c r="J15" s="66"/>
+        <v>800 x 458 px</v>
+      </c>
+      <c r="J15" s="66" t="s">
+        <v>199</v>
+      </c>
       <c r="K15" s="66"/>
       <c r="O15" s="2" t="str">
         <f>'Definición técnica de imagenes'!A24</f>
@@ -3131,33 +3078,41 @@
     </row>
     <row r="16" spans="1:16" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B16" s="62"/>
+        <f t="shared" si="1"/>
+        <v>IMG07</v>
+      </c>
+      <c r="B16" s="62" t="s">
+        <v>200</v>
+      </c>
       <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
+        <v>Recurso F6</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>194</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>155</v>
+      </c>
       <c r="F16" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="2"/>
+        <v>LE_08_03_REC190_IMG07n.jpg</v>
       </c>
       <c r="G16" s="13" t="str">
         <f ca="1">IF($F16&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>320 x 480 px</v>
       </c>
       <c r="H16" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
+        <f t="shared" ca="1" si="3"/>
+        <v>LE_08_03_REC190_IMG07a.jpg</v>
       </c>
       <c r="I16" s="13" t="str">
         <f ca="1">IF(OR($B16&lt;&gt;"",$J16&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v/>
-      </c>
-      <c r="J16" s="67"/>
+        <v>800 x 458 px</v>
+      </c>
+      <c r="J16" s="67" t="s">
+        <v>196</v>
+      </c>
       <c r="K16" s="68"/>
       <c r="O16" s="2" t="str">
         <f>'Definición técnica de imagenes'!A25</f>
@@ -3166,33 +3121,41 @@
     </row>
     <row r="17" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B17" s="62"/>
+        <f t="shared" si="1"/>
+        <v>IMG08</v>
+      </c>
+      <c r="B17" s="62" t="s">
+        <v>201</v>
+      </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
+        <v>Recurso F6</v>
+      </c>
+      <c r="D17" s="63" t="s">
+        <v>194</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>155</v>
+      </c>
       <c r="F17" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="2"/>
+        <v>LE_08_03_REC190_IMG08n.jpg</v>
       </c>
       <c r="G17" s="13" t="str">
         <f ca="1">IF($F17&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>320 x 480 px</v>
       </c>
       <c r="H17" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
+        <f t="shared" ca="1" si="3"/>
+        <v>LE_08_03_REC190_IMG08a.jpg</v>
       </c>
       <c r="I17" s="13" t="str">
         <f ca="1">IF(OR($B17&lt;&gt;"",$J17&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v/>
-      </c>
-      <c r="J17" s="66"/>
+        <v>800 x 458 px</v>
+      </c>
+      <c r="J17" s="66" t="s">
+        <v>202</v>
+      </c>
       <c r="K17" s="66"/>
       <c r="O17" s="2" t="str">
         <f>'Definición técnica de imagenes'!A27</f>
@@ -3201,33 +3164,41 @@
     </row>
     <row r="18" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B18" s="62"/>
+        <f t="shared" si="1"/>
+        <v>IMG09</v>
+      </c>
+      <c r="B18" s="62" t="s">
+        <v>203</v>
+      </c>
       <c r="C18" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
+        <v>Recurso F6</v>
+      </c>
+      <c r="D18" s="63" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>155</v>
+      </c>
       <c r="F18" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="2"/>
+        <v>LE_08_03_REC190_IMG09n.jpg</v>
       </c>
       <c r="G18" s="13" t="str">
         <f ca="1">IF($F18&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>320 x 480 px</v>
       </c>
       <c r="H18" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
+        <f t="shared" ca="1" si="3"/>
+        <v>LE_08_03_REC190_IMG09a.jpg</v>
       </c>
       <c r="I18" s="13" t="str">
         <f ca="1">IF(OR($B18&lt;&gt;"",$J18&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v/>
-      </c>
-      <c r="J18" s="66"/>
+        <v>800 x 458 px</v>
+      </c>
+      <c r="J18" s="66" t="s">
+        <v>204</v>
+      </c>
       <c r="K18" s="66"/>
       <c r="O18" s="2" t="str">
         <f>'Definición técnica de imagenes'!A30</f>
@@ -3236,7 +3207,7 @@
     </row>
     <row r="19" spans="1:15" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="str">
-        <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
+        <f t="shared" ref="A19:A50" si="4">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v/>
       </c>
       <c r="B19" s="62"/>
@@ -3247,7 +3218,7 @@
       <c r="D19" s="63"/>
       <c r="E19" s="63"/>
       <c r="F19" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G19" s="13" t="str">
@@ -3255,7 +3226,7 @@
         <v/>
       </c>
       <c r="H19" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I19" s="13" t="str">
@@ -3271,7 +3242,7 @@
     </row>
     <row r="20" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B20" s="62"/>
@@ -3282,7 +3253,7 @@
       <c r="D20" s="63"/>
       <c r="E20" s="63"/>
       <c r="F20" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G20" s="13" t="str">
@@ -3290,7 +3261,7 @@
         <v/>
       </c>
       <c r="H20" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I20" s="13" t="str">
@@ -3306,7 +3277,7 @@
     </row>
     <row r="21" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B21" s="62"/>
@@ -3317,7 +3288,7 @@
       <c r="D21" s="63"/>
       <c r="E21" s="63"/>
       <c r="F21" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G21" s="13" t="str">
@@ -3325,7 +3296,7 @@
         <v/>
       </c>
       <c r="H21" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I21" s="13" t="str">
@@ -3341,7 +3312,7 @@
     </row>
     <row r="22" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B22" s="62"/>
@@ -3352,7 +3323,7 @@
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
       <c r="F22" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G22" s="13" t="str">
@@ -3360,7 +3331,7 @@
         <v/>
       </c>
       <c r="H22" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I22" s="13" t="str">
@@ -3376,7 +3347,7 @@
     </row>
     <row r="23" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B23" s="62"/>
@@ -3387,7 +3358,7 @@
       <c r="D23" s="63"/>
       <c r="E23" s="63"/>
       <c r="F23" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G23" s="13" t="str">
@@ -3395,7 +3366,7 @@
         <v/>
       </c>
       <c r="H23" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I23" s="13" t="str">
@@ -3411,7 +3382,7 @@
     </row>
     <row r="24" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B24" s="62"/>
@@ -3422,7 +3393,7 @@
       <c r="D24" s="63"/>
       <c r="E24" s="63"/>
       <c r="F24" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G24" s="13" t="str">
@@ -3430,7 +3401,7 @@
         <v/>
       </c>
       <c r="H24" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I24" s="13" t="str">
@@ -3446,7 +3417,7 @@
     </row>
     <row r="25" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B25" s="62"/>
@@ -3457,7 +3428,7 @@
       <c r="D25" s="63"/>
       <c r="E25" s="63"/>
       <c r="F25" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G25" s="13" t="str">
@@ -3465,7 +3436,7 @@
         <v/>
       </c>
       <c r="H25" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I25" s="13" t="str">
@@ -3477,7 +3448,7 @@
     </row>
     <row r="26" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B26" s="62"/>
@@ -3488,7 +3459,7 @@
       <c r="D26" s="63"/>
       <c r="E26" s="63"/>
       <c r="F26" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G26" s="13" t="str">
@@ -3496,7 +3467,7 @@
         <v/>
       </c>
       <c r="H26" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I26" s="13" t="str">
@@ -3508,7 +3479,7 @@
     </row>
     <row r="27" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B27" s="62"/>
@@ -3519,7 +3490,7 @@
       <c r="D27" s="63"/>
       <c r="E27" s="63"/>
       <c r="F27" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G27" s="13" t="str">
@@ -3527,7 +3498,7 @@
         <v/>
       </c>
       <c r="H27" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I27" s="13" t="str">
@@ -3540,7 +3511,7 @@
     </row>
     <row r="28" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B28" s="62"/>
@@ -3551,7 +3522,7 @@
       <c r="D28" s="63"/>
       <c r="E28" s="63"/>
       <c r="F28" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G28" s="13" t="str">
@@ -3559,7 +3530,7 @@
         <v/>
       </c>
       <c r="H28" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I28" s="13" t="str">
@@ -3571,7 +3542,7 @@
     </row>
     <row r="29" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B29" s="62"/>
@@ -3582,7 +3553,7 @@
       <c r="D29" s="63"/>
       <c r="E29" s="63"/>
       <c r="F29" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G29" s="13" t="str">
@@ -3590,7 +3561,7 @@
         <v/>
       </c>
       <c r="H29" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I29" s="13" t="str">
@@ -3602,7 +3573,7 @@
     </row>
     <row r="30" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B30" s="62"/>
@@ -3613,7 +3584,7 @@
       <c r="D30" s="63"/>
       <c r="E30" s="63"/>
       <c r="F30" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G30" s="13" t="str">
@@ -3621,7 +3592,7 @@
         <v/>
       </c>
       <c r="H30" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I30" s="13" t="str">
@@ -3633,7 +3604,7 @@
     </row>
     <row r="31" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B31" s="62"/>
@@ -3644,7 +3615,7 @@
       <c r="D31" s="63"/>
       <c r="E31" s="63"/>
       <c r="F31" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G31" s="13" t="str">
@@ -3652,7 +3623,7 @@
         <v/>
       </c>
       <c r="H31" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I31" s="13" t="str">
@@ -3664,7 +3635,7 @@
     </row>
     <row r="32" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B32" s="62"/>
@@ -3675,7 +3646,7 @@
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
       <c r="F32" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G32" s="13" t="str">
@@ -3683,7 +3654,7 @@
         <v/>
       </c>
       <c r="H32" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I32" s="13" t="str">
@@ -3695,7 +3666,7 @@
     </row>
     <row r="33" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B33" s="62"/>
@@ -3706,7 +3677,7 @@
       <c r="D33" s="63"/>
       <c r="E33" s="63"/>
       <c r="F33" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G33" s="13" t="str">
@@ -3714,7 +3685,7 @@
         <v/>
       </c>
       <c r="H33" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I33" s="13" t="str">
@@ -3726,7 +3697,7 @@
     </row>
     <row r="34" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B34" s="62"/>
@@ -3737,7 +3708,7 @@
       <c r="D34" s="63"/>
       <c r="E34" s="63"/>
       <c r="F34" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G34" s="13" t="str">
@@ -3745,7 +3716,7 @@
         <v/>
       </c>
       <c r="H34" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I34" s="13" t="str">
@@ -3758,7 +3729,7 @@
     </row>
     <row r="35" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B35" s="62"/>
@@ -3769,7 +3740,7 @@
       <c r="D35" s="63"/>
       <c r="E35" s="63"/>
       <c r="F35" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G35" s="13" t="str">
@@ -3777,7 +3748,7 @@
         <v/>
       </c>
       <c r="H35" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I35" s="13" t="str">
@@ -3790,7 +3761,7 @@
     </row>
     <row r="36" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B36" s="62"/>
@@ -3801,7 +3772,7 @@
       <c r="D36" s="63"/>
       <c r="E36" s="63"/>
       <c r="F36" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G36" s="13" t="str">
@@ -3809,7 +3780,7 @@
         <v/>
       </c>
       <c r="H36" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I36" s="13" t="str">
@@ -3822,7 +3793,7 @@
     </row>
     <row r="37" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B37" s="62"/>
@@ -3833,7 +3804,7 @@
       <c r="D37" s="63"/>
       <c r="E37" s="63"/>
       <c r="F37" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G37" s="13" t="str">
@@ -3841,7 +3812,7 @@
         <v/>
       </c>
       <c r="H37" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I37" s="13" t="str">
@@ -3853,7 +3824,7 @@
     </row>
     <row r="38" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B38" s="62"/>
@@ -3864,7 +3835,7 @@
       <c r="D38" s="63"/>
       <c r="E38" s="63"/>
       <c r="F38" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G38" s="13" t="str">
@@ -3872,7 +3843,7 @@
         <v/>
       </c>
       <c r="H38" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I38" s="13" t="str">
@@ -3884,7 +3855,7 @@
     </row>
     <row r="39" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B39" s="62"/>
@@ -3895,7 +3866,7 @@
       <c r="D39" s="63"/>
       <c r="E39" s="63"/>
       <c r="F39" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G39" s="13" t="str">
@@ -3903,7 +3874,7 @@
         <v/>
       </c>
       <c r="H39" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I39" s="13" t="str">
@@ -3915,7 +3886,7 @@
     </row>
     <row r="40" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B40" s="62"/>
@@ -3926,7 +3897,7 @@
       <c r="D40" s="63"/>
       <c r="E40" s="63"/>
       <c r="F40" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G40" s="13" t="str">
@@ -3934,7 +3905,7 @@
         <v/>
       </c>
       <c r="H40" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I40" s="13" t="str">
@@ -3946,7 +3917,7 @@
     </row>
     <row r="41" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B41" s="62"/>
@@ -3957,7 +3928,7 @@
       <c r="D41" s="63"/>
       <c r="E41" s="63"/>
       <c r="F41" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G41" s="13" t="str">
@@ -3965,7 +3936,7 @@
         <v/>
       </c>
       <c r="H41" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I41" s="13" t="str">
@@ -3977,18 +3948,18 @@
     </row>
     <row r="42" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B42" s="62"/>
       <c r="C42" s="20" t="str">
-        <f t="shared" ref="C42:C73" si="7">IF(OR(B42&lt;&gt;"",J42&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f t="shared" ref="C42:C73" si="5">IF(OR(B42&lt;&gt;"",J42&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v/>
       </c>
       <c r="D42" s="63"/>
       <c r="E42" s="63"/>
       <c r="F42" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G42" s="13" t="str">
@@ -3996,7 +3967,7 @@
         <v/>
       </c>
       <c r="H42" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I42" s="13" t="str">
@@ -4008,18 +3979,18 @@
     </row>
     <row r="43" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B43" s="62"/>
       <c r="C43" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D43" s="63"/>
       <c r="E43" s="63"/>
       <c r="F43" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G43" s="13" t="str">
@@ -4027,7 +3998,7 @@
         <v/>
       </c>
       <c r="H43" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I43" s="13" t="str">
@@ -4039,18 +4010,18 @@
     </row>
     <row r="44" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B44" s="62"/>
       <c r="C44" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D44" s="63"/>
       <c r="E44" s="63"/>
       <c r="F44" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G44" s="13" t="str">
@@ -4058,7 +4029,7 @@
         <v/>
       </c>
       <c r="H44" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I44" s="13" t="str">
@@ -4070,18 +4041,18 @@
     </row>
     <row r="45" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B45" s="62"/>
       <c r="C45" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D45" s="63"/>
       <c r="E45" s="63"/>
       <c r="F45" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G45" s="13" t="str">
@@ -4089,7 +4060,7 @@
         <v/>
       </c>
       <c r="H45" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I45" s="13" t="str">
@@ -4101,18 +4072,18 @@
     </row>
     <row r="46" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B46" s="62"/>
       <c r="C46" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D46" s="63"/>
       <c r="E46" s="63"/>
       <c r="F46" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G46" s="13" t="str">
@@ -4120,7 +4091,7 @@
         <v/>
       </c>
       <c r="H46" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I46" s="13" t="str">
@@ -4132,18 +4103,18 @@
     </row>
     <row r="47" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B47" s="62"/>
       <c r="C47" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D47" s="63"/>
       <c r="E47" s="63"/>
       <c r="F47" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G47" s="13" t="str">
@@ -4151,7 +4122,7 @@
         <v/>
       </c>
       <c r="H47" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I47" s="13" t="str">
@@ -4163,18 +4134,18 @@
     </row>
     <row r="48" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B48" s="62"/>
       <c r="C48" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D48" s="63"/>
       <c r="E48" s="63"/>
       <c r="F48" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G48" s="13" t="str">
@@ -4182,7 +4153,7 @@
         <v/>
       </c>
       <c r="H48" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I48" s="13" t="str">
@@ -4194,18 +4165,18 @@
     </row>
     <row r="49" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B49" s="62"/>
       <c r="C49" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D49" s="63"/>
       <c r="E49" s="63"/>
       <c r="F49" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G49" s="13" t="str">
@@ -4213,7 +4184,7 @@
         <v/>
       </c>
       <c r="H49" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I49" s="13" t="str">
@@ -4225,18 +4196,18 @@
     </row>
     <row r="50" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B50" s="62"/>
       <c r="C50" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D50" s="63"/>
       <c r="E50" s="63"/>
       <c r="F50" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G50" s="13" t="str">
@@ -4244,7 +4215,7 @@
         <v/>
       </c>
       <c r="H50" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I50" s="13" t="str">
@@ -4256,18 +4227,18 @@
     </row>
     <row r="51" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="str">
-        <f t="shared" ref="A51:A82" si="8">IF(OR(B51&lt;&gt;"",J51&lt;&gt;""),CONCATENATE(LEFT(A50,3),IF(MID(A50,4,2)+1&lt;10,CONCATENATE("0",MID(A50,4,2)+1),MID(A50,4,2)+1)),"")</f>
+        <f t="shared" ref="A51:A82" si="6">IF(OR(B51&lt;&gt;"",J51&lt;&gt;""),CONCATENATE(LEFT(A50,3),IF(MID(A50,4,2)+1&lt;10,CONCATENATE("0",MID(A50,4,2)+1),MID(A50,4,2)+1)),"")</f>
         <v/>
       </c>
       <c r="B51" s="62"/>
       <c r="C51" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D51" s="63"/>
       <c r="E51" s="63"/>
       <c r="F51" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G51" s="13" t="str">
@@ -4275,7 +4246,7 @@
         <v/>
       </c>
       <c r="H51" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I51" s="13" t="str">
@@ -4287,18 +4258,18 @@
     </row>
     <row r="52" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B52" s="62"/>
       <c r="C52" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D52" s="63"/>
       <c r="E52" s="63"/>
       <c r="F52" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G52" s="13" t="str">
@@ -4306,7 +4277,7 @@
         <v/>
       </c>
       <c r="H52" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I52" s="13" t="str">
@@ -4318,18 +4289,18 @@
     </row>
     <row r="53" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B53" s="62"/>
       <c r="C53" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D53" s="63"/>
       <c r="E53" s="63"/>
       <c r="F53" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G53" s="13" t="str">
@@ -4337,7 +4308,7 @@
         <v/>
       </c>
       <c r="H53" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I53" s="13" t="str">
@@ -4349,18 +4320,18 @@
     </row>
     <row r="54" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B54" s="62"/>
       <c r="C54" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D54" s="63"/>
       <c r="E54" s="63"/>
       <c r="F54" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G54" s="13" t="str">
@@ -4368,7 +4339,7 @@
         <v/>
       </c>
       <c r="H54" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I54" s="13" t="str">
@@ -4380,18 +4351,18 @@
     </row>
     <row r="55" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B55" s="62"/>
       <c r="C55" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D55" s="63"/>
       <c r="E55" s="63"/>
       <c r="F55" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G55" s="13" t="str">
@@ -4399,7 +4370,7 @@
         <v/>
       </c>
       <c r="H55" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I55" s="13" t="str">
@@ -4411,18 +4382,18 @@
     </row>
     <row r="56" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B56" s="62"/>
       <c r="C56" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D56" s="63"/>
       <c r="E56" s="63"/>
       <c r="F56" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G56" s="13" t="str">
@@ -4430,7 +4401,7 @@
         <v/>
       </c>
       <c r="H56" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I56" s="13" t="str">
@@ -4442,18 +4413,18 @@
     </row>
     <row r="57" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B57" s="62"/>
       <c r="C57" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D57" s="63"/>
       <c r="E57" s="63"/>
       <c r="F57" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G57" s="13" t="str">
@@ -4461,7 +4432,7 @@
         <v/>
       </c>
       <c r="H57" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I57" s="13" t="str">
@@ -4473,18 +4444,18 @@
     </row>
     <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B58" s="62"/>
       <c r="C58" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D58" s="63"/>
       <c r="E58" s="63"/>
       <c r="F58" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G58" s="13" t="str">
@@ -4492,7 +4463,7 @@
         <v/>
       </c>
       <c r="H58" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I58" s="13" t="str">
@@ -4504,18 +4475,18 @@
     </row>
     <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B59" s="62"/>
       <c r="C59" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D59" s="63"/>
       <c r="E59" s="63"/>
       <c r="F59" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G59" s="13" t="str">
@@ -4523,7 +4494,7 @@
         <v/>
       </c>
       <c r="H59" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I59" s="13" t="str">
@@ -4535,18 +4506,18 @@
     </row>
     <row r="60" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B60" s="62"/>
       <c r="C60" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D60" s="63"/>
       <c r="E60" s="63"/>
       <c r="F60" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G60" s="13" t="str">
@@ -4554,7 +4525,7 @@
         <v/>
       </c>
       <c r="H60" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I60" s="13" t="str">
@@ -4566,18 +4537,18 @@
     </row>
     <row r="61" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B61" s="62"/>
       <c r="C61" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D61" s="63"/>
       <c r="E61" s="63"/>
       <c r="F61" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G61" s="13" t="str">
@@ -4585,7 +4556,7 @@
         <v/>
       </c>
       <c r="H61" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I61" s="13" t="str">
@@ -4597,18 +4568,18 @@
     </row>
     <row r="62" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B62" s="62"/>
       <c r="C62" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D62" s="63"/>
       <c r="E62" s="63"/>
       <c r="F62" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G62" s="13" t="str">
@@ -4616,7 +4587,7 @@
         <v/>
       </c>
       <c r="H62" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I62" s="13" t="str">
@@ -4628,18 +4599,18 @@
     </row>
     <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B63" s="62"/>
       <c r="C63" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D63" s="63"/>
       <c r="E63" s="63"/>
       <c r="F63" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G63" s="13" t="str">
@@ -4647,7 +4618,7 @@
         <v/>
       </c>
       <c r="H63" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I63" s="13" t="str">
@@ -4659,18 +4630,18 @@
     </row>
     <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B64" s="62"/>
       <c r="C64" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D64" s="63"/>
       <c r="E64" s="63"/>
       <c r="F64" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G64" s="13" t="str">
@@ -4678,7 +4649,7 @@
         <v/>
       </c>
       <c r="H64" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I64" s="13" t="str">
@@ -4690,18 +4661,18 @@
     </row>
     <row r="65" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B65" s="62"/>
       <c r="C65" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D65" s="63"/>
       <c r="E65" s="63"/>
       <c r="F65" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G65" s="13" t="str">
@@ -4709,7 +4680,7 @@
         <v/>
       </c>
       <c r="H65" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I65" s="13" t="str">
@@ -4721,18 +4692,18 @@
     </row>
     <row r="66" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B66" s="62"/>
       <c r="C66" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D66" s="63"/>
       <c r="E66" s="63"/>
       <c r="F66" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G66" s="13" t="str">
@@ -4740,7 +4711,7 @@
         <v/>
       </c>
       <c r="H66" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I66" s="13" t="str">
@@ -4752,18 +4723,18 @@
     </row>
     <row r="67" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B67" s="62"/>
       <c r="C67" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D67" s="63"/>
       <c r="E67" s="63"/>
       <c r="F67" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G67" s="13" t="str">
@@ -4771,7 +4742,7 @@
         <v/>
       </c>
       <c r="H67" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I67" s="13" t="str">
@@ -4783,18 +4754,18 @@
     </row>
     <row r="68" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B68" s="62"/>
       <c r="C68" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D68" s="63"/>
       <c r="E68" s="63"/>
       <c r="F68" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G68" s="13" t="str">
@@ -4802,7 +4773,7 @@
         <v/>
       </c>
       <c r="H68" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I68" s="13" t="str">
@@ -4814,18 +4785,18 @@
     </row>
     <row r="69" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B69" s="62"/>
       <c r="C69" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D69" s="63"/>
       <c r="E69" s="63"/>
       <c r="F69" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G69" s="13" t="str">
@@ -4833,7 +4804,7 @@
         <v/>
       </c>
       <c r="H69" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I69" s="13" t="str">
@@ -4845,18 +4816,18 @@
     </row>
     <row r="70" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B70" s="62"/>
       <c r="C70" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D70" s="63"/>
       <c r="E70" s="63"/>
       <c r="F70" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G70" s="13" t="str">
@@ -4864,7 +4835,7 @@
         <v/>
       </c>
       <c r="H70" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I70" s="13" t="str">
@@ -4876,18 +4847,18 @@
     </row>
     <row r="71" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B71" s="62"/>
       <c r="C71" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D71" s="63"/>
       <c r="E71" s="63"/>
       <c r="F71" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G71" s="13" t="str">
@@ -4895,7 +4866,7 @@
         <v/>
       </c>
       <c r="H71" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I71" s="13" t="str">
@@ -4907,18 +4878,18 @@
     </row>
     <row r="72" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B72" s="62"/>
       <c r="C72" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D72" s="63"/>
       <c r="E72" s="63"/>
       <c r="F72" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G72" s="13" t="str">
@@ -4926,7 +4897,7 @@
         <v/>
       </c>
       <c r="H72" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I72" s="13" t="str">
@@ -4938,18 +4909,18 @@
     </row>
     <row r="73" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B73" s="62"/>
       <c r="C73" s="20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D73" s="63"/>
       <c r="E73" s="63"/>
       <c r="F73" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G73" s="13" t="str">
@@ -4957,7 +4928,7 @@
         <v/>
       </c>
       <c r="H73" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I73" s="13" t="str">
@@ -4969,18 +4940,18 @@
     </row>
     <row r="74" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B74" s="62"/>
       <c r="C74" s="20" t="str">
-        <f t="shared" ref="C74:C105" si="9">IF(OR(B74&lt;&gt;"",J74&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f t="shared" ref="C74:C105" si="7">IF(OR(B74&lt;&gt;"",J74&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v/>
       </c>
       <c r="D74" s="63"/>
       <c r="E74" s="63"/>
       <c r="F74" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G74" s="13" t="str">
@@ -4988,7 +4959,7 @@
         <v/>
       </c>
       <c r="H74" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="I74" s="13" t="str">
@@ -5000,18 +4971,18 @@
     </row>
     <row r="75" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B75" s="62"/>
       <c r="C75" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D75" s="63"/>
       <c r="E75" s="63"/>
       <c r="F75" s="13" t="str">
-        <f t="shared" ref="F75:F108" si="10">IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I75="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" ref="F75:F108" si="8">IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I75="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v/>
       </c>
       <c r="G75" s="13" t="str">
@@ -5019,7 +4990,7 @@
         <v/>
       </c>
       <c r="H75" s="13" t="str">
-        <f t="shared" ref="H75:H108" ca="1" si="11">IF(AND(I75&lt;&gt;"",I75&lt;&gt;0),IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" ref="H75:H108" ca="1" si="9">IF(AND(I75&lt;&gt;"",I75&lt;&gt;0),IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I75" s="13" t="str">
@@ -5031,18 +5002,18 @@
     </row>
     <row r="76" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B76" s="62"/>
       <c r="C76" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D76" s="63"/>
       <c r="E76" s="63"/>
       <c r="F76" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G76" s="13" t="str">
@@ -5050,7 +5021,7 @@
         <v/>
       </c>
       <c r="H76" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I76" s="13" t="str">
@@ -5062,18 +5033,18 @@
     </row>
     <row r="77" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B77" s="62"/>
       <c r="C77" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D77" s="63"/>
       <c r="E77" s="63"/>
       <c r="F77" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G77" s="13" t="str">
@@ -5081,7 +5052,7 @@
         <v/>
       </c>
       <c r="H77" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I77" s="13" t="str">
@@ -5093,18 +5064,18 @@
     </row>
     <row r="78" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B78" s="62"/>
       <c r="C78" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D78" s="63"/>
       <c r="E78" s="63"/>
       <c r="F78" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G78" s="13" t="str">
@@ -5112,7 +5083,7 @@
         <v/>
       </c>
       <c r="H78" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I78" s="13" t="str">
@@ -5124,18 +5095,18 @@
     </row>
     <row r="79" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B79" s="62"/>
       <c r="C79" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D79" s="63"/>
       <c r="E79" s="63"/>
       <c r="F79" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G79" s="13" t="str">
@@ -5143,7 +5114,7 @@
         <v/>
       </c>
       <c r="H79" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I79" s="13" t="str">
@@ -5155,18 +5126,18 @@
     </row>
     <row r="80" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B80" s="62"/>
       <c r="C80" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D80" s="63"/>
       <c r="E80" s="63"/>
       <c r="F80" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G80" s="13" t="str">
@@ -5174,7 +5145,7 @@
         <v/>
       </c>
       <c r="H80" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I80" s="13" t="str">
@@ -5186,18 +5157,18 @@
     </row>
     <row r="81" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B81" s="62"/>
       <c r="C81" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D81" s="63"/>
       <c r="E81" s="63"/>
       <c r="F81" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G81" s="13" t="str">
@@ -5205,7 +5176,7 @@
         <v/>
       </c>
       <c r="H81" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I81" s="13" t="str">
@@ -5217,18 +5188,18 @@
     </row>
     <row r="82" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B82" s="62"/>
       <c r="C82" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D82" s="63"/>
       <c r="E82" s="63"/>
       <c r="F82" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G82" s="13" t="str">
@@ -5236,7 +5207,7 @@
         <v/>
       </c>
       <c r="H82" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I82" s="13" t="str">
@@ -5248,18 +5219,18 @@
     </row>
     <row r="83" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="str">
-        <f t="shared" ref="A83:A108" si="12">IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),CONCATENATE(LEFT(A82,3),IF(MID(A82,4,2)+1&lt;10,CONCATENATE("0",MID(A82,4,2)+1),MID(A82,4,2)+1)),"")</f>
+        <f t="shared" ref="A83:A108" si="10">IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),CONCATENATE(LEFT(A82,3),IF(MID(A82,4,2)+1&lt;10,CONCATENATE("0",MID(A82,4,2)+1),MID(A82,4,2)+1)),"")</f>
         <v/>
       </c>
       <c r="B83" s="62"/>
       <c r="C83" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D83" s="63"/>
       <c r="E83" s="63"/>
       <c r="F83" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G83" s="13" t="str">
@@ -5267,7 +5238,7 @@
         <v/>
       </c>
       <c r="H83" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I83" s="13" t="str">
@@ -5279,18 +5250,18 @@
     </row>
     <row r="84" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B84" s="62"/>
       <c r="C84" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D84" s="63"/>
       <c r="E84" s="63"/>
       <c r="F84" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G84" s="13" t="str">
@@ -5298,7 +5269,7 @@
         <v/>
       </c>
       <c r="H84" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I84" s="13" t="str">
@@ -5310,18 +5281,18 @@
     </row>
     <row r="85" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B85" s="62"/>
       <c r="C85" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D85" s="63"/>
       <c r="E85" s="63"/>
       <c r="F85" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G85" s="13" t="str">
@@ -5329,7 +5300,7 @@
         <v/>
       </c>
       <c r="H85" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I85" s="13" t="str">
@@ -5341,18 +5312,18 @@
     </row>
     <row r="86" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B86" s="62"/>
       <c r="C86" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D86" s="63"/>
       <c r="E86" s="63"/>
       <c r="F86" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G86" s="13" t="str">
@@ -5360,7 +5331,7 @@
         <v/>
       </c>
       <c r="H86" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I86" s="13" t="str">
@@ -5372,18 +5343,18 @@
     </row>
     <row r="87" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B87" s="62"/>
       <c r="C87" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D87" s="63"/>
       <c r="E87" s="63"/>
       <c r="F87" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G87" s="13" t="str">
@@ -5391,7 +5362,7 @@
         <v/>
       </c>
       <c r="H87" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I87" s="13" t="str">
@@ -5403,18 +5374,18 @@
     </row>
     <row r="88" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B88" s="62"/>
       <c r="C88" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D88" s="63"/>
       <c r="E88" s="63"/>
       <c r="F88" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G88" s="13" t="str">
@@ -5422,7 +5393,7 @@
         <v/>
       </c>
       <c r="H88" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I88" s="13" t="str">
@@ -5434,18 +5405,18 @@
     </row>
     <row r="89" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B89" s="62"/>
       <c r="C89" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D89" s="63"/>
       <c r="E89" s="63"/>
       <c r="F89" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G89" s="13" t="str">
@@ -5453,7 +5424,7 @@
         <v/>
       </c>
       <c r="H89" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I89" s="13" t="str">
@@ -5465,18 +5436,18 @@
     </row>
     <row r="90" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B90" s="62"/>
       <c r="C90" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D90" s="63"/>
       <c r="E90" s="63"/>
       <c r="F90" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G90" s="13" t="str">
@@ -5484,7 +5455,7 @@
         <v/>
       </c>
       <c r="H90" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I90" s="13" t="str">
@@ -5496,18 +5467,18 @@
     </row>
     <row r="91" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B91" s="62"/>
       <c r="C91" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D91" s="63"/>
       <c r="E91" s="63"/>
       <c r="F91" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G91" s="13" t="str">
@@ -5515,7 +5486,7 @@
         <v/>
       </c>
       <c r="H91" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I91" s="13" t="str">
@@ -5527,18 +5498,18 @@
     </row>
     <row r="92" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B92" s="62"/>
       <c r="C92" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D92" s="63"/>
       <c r="E92" s="63"/>
       <c r="F92" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G92" s="13" t="str">
@@ -5546,7 +5517,7 @@
         <v/>
       </c>
       <c r="H92" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I92" s="13" t="str">
@@ -5558,18 +5529,18 @@
     </row>
     <row r="93" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B93" s="62"/>
       <c r="C93" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D93" s="63"/>
       <c r="E93" s="63"/>
       <c r="F93" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G93" s="13" t="str">
@@ -5577,7 +5548,7 @@
         <v/>
       </c>
       <c r="H93" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I93" s="13" t="str">
@@ -5589,18 +5560,18 @@
     </row>
     <row r="94" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B94" s="62"/>
       <c r="C94" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D94" s="63"/>
       <c r="E94" s="63"/>
       <c r="F94" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G94" s="13" t="str">
@@ -5608,7 +5579,7 @@
         <v/>
       </c>
       <c r="H94" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I94" s="13" t="str">
@@ -5620,18 +5591,18 @@
     </row>
     <row r="95" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B95" s="62"/>
       <c r="C95" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D95" s="63"/>
       <c r="E95" s="63"/>
       <c r="F95" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G95" s="13" t="str">
@@ -5639,7 +5610,7 @@
         <v/>
       </c>
       <c r="H95" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I95" s="13" t="str">
@@ -5651,18 +5622,18 @@
     </row>
     <row r="96" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B96" s="62"/>
       <c r="C96" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D96" s="63"/>
       <c r="E96" s="63"/>
       <c r="F96" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G96" s="13" t="str">
@@ -5670,7 +5641,7 @@
         <v/>
       </c>
       <c r="H96" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I96" s="13" t="str">
@@ -5682,18 +5653,18 @@
     </row>
     <row r="97" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B97" s="62"/>
       <c r="C97" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D97" s="63"/>
       <c r="E97" s="63"/>
       <c r="F97" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G97" s="13" t="str">
@@ -5701,7 +5672,7 @@
         <v/>
       </c>
       <c r="H97" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I97" s="13" t="str">
@@ -5713,18 +5684,18 @@
     </row>
     <row r="98" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B98" s="62"/>
       <c r="C98" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D98" s="63"/>
       <c r="E98" s="63"/>
       <c r="F98" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G98" s="13" t="str">
@@ -5732,7 +5703,7 @@
         <v/>
       </c>
       <c r="H98" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I98" s="13" t="str">
@@ -5744,18 +5715,18 @@
     </row>
     <row r="99" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B99" s="62"/>
       <c r="C99" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D99" s="63"/>
       <c r="E99" s="63"/>
       <c r="F99" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G99" s="13" t="str">
@@ -5763,7 +5734,7 @@
         <v/>
       </c>
       <c r="H99" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I99" s="13" t="str">
@@ -5775,18 +5746,18 @@
     </row>
     <row r="100" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B100" s="62"/>
       <c r="C100" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D100" s="63"/>
       <c r="E100" s="63"/>
       <c r="F100" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G100" s="13" t="str">
@@ -5794,7 +5765,7 @@
         <v/>
       </c>
       <c r="H100" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I100" s="13" t="str">
@@ -5806,18 +5777,18 @@
     </row>
     <row r="101" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B101" s="62"/>
       <c r="C101" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D101" s="63"/>
       <c r="E101" s="63"/>
       <c r="F101" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G101" s="13" t="str">
@@ -5825,7 +5796,7 @@
         <v/>
       </c>
       <c r="H101" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I101" s="13" t="str">
@@ -5837,18 +5808,18 @@
     </row>
     <row r="102" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B102" s="62"/>
       <c r="C102" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D102" s="63"/>
       <c r="E102" s="63"/>
       <c r="F102" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G102" s="13" t="str">
@@ -5856,7 +5827,7 @@
         <v/>
       </c>
       <c r="H102" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I102" s="13" t="str">
@@ -5868,18 +5839,18 @@
     </row>
     <row r="103" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B103" s="62"/>
       <c r="C103" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D103" s="63"/>
       <c r="E103" s="63"/>
       <c r="F103" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G103" s="13" t="str">
@@ -5887,7 +5858,7 @@
         <v/>
       </c>
       <c r="H103" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I103" s="13" t="str">
@@ -5899,18 +5870,18 @@
     </row>
     <row r="104" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B104" s="62"/>
       <c r="C104" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D104" s="63"/>
       <c r="E104" s="63"/>
       <c r="F104" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G104" s="13" t="str">
@@ -5918,7 +5889,7 @@
         <v/>
       </c>
       <c r="H104" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I104" s="13" t="str">
@@ -5930,18 +5901,18 @@
     </row>
     <row r="105" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B105" s="62"/>
       <c r="C105" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D105" s="63"/>
       <c r="E105" s="63"/>
       <c r="F105" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G105" s="13" t="str">
@@ -5949,7 +5920,7 @@
         <v/>
       </c>
       <c r="H105" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I105" s="13" t="str">
@@ -5961,7 +5932,7 @@
     </row>
     <row r="106" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B106" s="62"/>
@@ -5972,7 +5943,7 @@
       <c r="D106" s="63"/>
       <c r="E106" s="63"/>
       <c r="F106" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G106" s="13" t="str">
@@ -5980,7 +5951,7 @@
         <v/>
       </c>
       <c r="H106" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I106" s="13" t="str">
@@ -5992,7 +5963,7 @@
     </row>
     <row r="107" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B107" s="62"/>
@@ -6003,7 +5974,7 @@
       <c r="D107" s="63"/>
       <c r="E107" s="63"/>
       <c r="F107" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G107" s="13" t="str">
@@ -6011,7 +5982,7 @@
         <v/>
       </c>
       <c r="H107" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I107" s="13" t="str">
@@ -6023,7 +5994,7 @@
     </row>
     <row r="108" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="B108" s="62"/>
@@ -6034,7 +6005,7 @@
       <c r="D108" s="63"/>
       <c r="E108" s="63"/>
       <c r="F108" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G108" s="13" t="str">
@@ -6042,7 +6013,7 @@
         <v/>
       </c>
       <c r="H108" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="I108" s="13" t="str">
@@ -6094,7 +6065,6 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6107,15 +6077,15 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.25" style="22" customWidth="1"/>
-    <col min="2" max="2" width="11" style="22"/>
+    <col min="1" max="1" width="72.125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="22"/>
     <col min="3" max="3" width="13.875" style="22" customWidth="1"/>
     <col min="4" max="4" width="11.375" style="22" customWidth="1"/>
-    <col min="5" max="7" width="11" style="22"/>
+    <col min="5" max="7" width="10.875" style="22"/>
     <col min="8" max="11" width="11" style="22" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="22"/>
+    <col min="12" max="16384" width="10.875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6401,7 +6371,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="66.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>47</v>
       </c>
@@ -6700,7 +6670,7 @@
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>828675</xdr:colOff>
+                    <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
                     <xdr:rowOff>714375</xdr:rowOff>
                   </to>
@@ -6716,7 +6686,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
                     <xdr:rowOff>485775</xdr:rowOff>
                   </from>
@@ -6738,7 +6708,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
                     <xdr:rowOff>485775</xdr:rowOff>
                   </from>
@@ -6760,15 +6730,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>1038225</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>228600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6782,15 +6752,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1047750</xdr:colOff>
+                    <xdr:colOff>1057275</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>866775</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>228600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6804,15 +6774,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>9525</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>0</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>228600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6837,14 +6807,14 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="22" customWidth="1"/>
-    <col min="2" max="2" width="24.25" style="22" customWidth="1"/>
+    <col min="2" max="2" width="24.125" style="22" customWidth="1"/>
     <col min="3" max="3" width="17" style="22" customWidth="1"/>
-    <col min="4" max="4" width="12.75" style="22" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="22" customWidth="1"/>
     <col min="5" max="5" width="6.875" style="22" customWidth="1"/>
     <col min="6" max="6" width="12.875" style="22" customWidth="1"/>
-    <col min="7" max="7" width="12.75" style="22" customWidth="1"/>
+    <col min="7" max="7" width="12.625" style="22" customWidth="1"/>
     <col min="8" max="8" width="24.5" style="22" customWidth="1"/>
-    <col min="9" max="9" width="27.25" style="22" customWidth="1"/>
+    <col min="9" max="9" width="27.125" style="22" customWidth="1"/>
     <col min="10" max="10" width="44.5" style="22" customWidth="1"/>
     <col min="11" max="16384" width="10.875" style="22"/>
   </cols>
@@ -6891,7 +6861,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>69</v>
       </c>
@@ -6916,7 +6886,7 @@
       </c>
       <c r="I3" s="40"/>
     </row>
-    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>57</v>
       </c>
@@ -6945,7 +6915,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>77</v>
       </c>
@@ -6974,7 +6944,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
         <v>58</v>
       </c>
@@ -7003,7 +6973,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
         <v>58</v>
       </c>
@@ -7028,7 +6998,7 @@
       </c>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
         <v>80</v>
       </c>
@@ -7057,7 +7027,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
         <v>82</v>
       </c>
@@ -7086,7 +7056,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
         <v>84</v>
       </c>
@@ -7115,7 +7085,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42" t="s">
         <v>86</v>
       </c>
@@ -7140,7 +7110,7 @@
       </c>
       <c r="I11" s="42"/>
     </row>
-    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
         <v>89</v>
       </c>
@@ -7169,7 +7139,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="42" t="s">
         <v>91</v>
       </c>
@@ -7198,7 +7168,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>94</v>
       </c>
@@ -7221,7 +7191,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="77" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="77" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="75" t="s">
         <v>96</v>
       </c>
@@ -7247,7 +7217,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
         <v>100</v>
       </c>
@@ -7275,7 +7245,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
         <v>103</v>
       </c>
@@ -7303,7 +7273,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
         <v>184</v>
       </c>
@@ -7329,7 +7299,7 @@
       <c r="I18" s="44"/>
       <c r="J18" s="49"/>
     </row>
-    <row r="19" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
         <v>137</v>
       </c>
@@ -7353,7 +7323,7 @@
       <c r="I19" s="44"/>
       <c r="J19" s="49"/>
     </row>
-    <row r="20" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
         <v>137</v>
       </c>
@@ -7377,7 +7347,7 @@
       <c r="I20" s="44"/>
       <c r="J20" s="49"/>
     </row>
-    <row r="21" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
         <v>137</v>
       </c>
@@ -7401,7 +7371,7 @@
       <c r="I21" s="72"/>
       <c r="J21" s="49"/>
     </row>
-    <row r="22" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="s">
         <v>132</v>
       </c>
@@ -7425,7 +7395,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
         <v>132</v>
       </c>
@@ -7454,7 +7424,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
         <v>134</v>
       </c>
@@ -7477,7 +7447,7 @@
       <c r="H24" s="44"/>
       <c r="I24" s="72"/>
     </row>
-    <row r="25" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="42" t="s">
         <v>135</v>
       </c>
@@ -7501,7 +7471,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
         <v>135</v>
       </c>
@@ -7530,7 +7500,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="42" t="s">
         <v>138</v>
       </c>
@@ -7554,7 +7524,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="42" t="s">
         <v>138</v>
       </c>
@@ -7578,7 +7548,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
         <v>138</v>
       </c>
@@ -7607,7 +7577,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
         <v>139</v>
       </c>
@@ -7630,7 +7600,7 @@
       <c r="H30" s="44"/>
       <c r="I30" s="44"/>
     </row>
-    <row r="31" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
         <v>140</v>
       </c>
@@ -7647,7 +7617,7 @@
       <c r="H31" s="44"/>
       <c r="I31" s="44"/>
     </row>
-    <row r="32" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
         <v>141</v>
       </c>
@@ -7662,7 +7632,7 @@
       <c r="H32" s="44"/>
       <c r="I32" s="44"/>
     </row>
-    <row r="33" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
         <v>136</v>
       </c>
@@ -7683,7 +7653,7 @@
       <c r="H33" s="44"/>
       <c r="I33" s="44"/>
     </row>
-    <row r="34" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
         <v>142</v>
       </c>
@@ -7700,7 +7670,7 @@
       <c r="H34" s="44"/>
       <c r="I34" s="44"/>
     </row>
-    <row r="35" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="42" t="s">
         <v>95</v>
       </c>
@@ -7729,7 +7699,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>95</v>
       </c>
@@ -7758,7 +7728,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="42" t="s">
         <v>143</v>
       </c>
@@ -7781,7 +7751,7 @@
       <c r="H37" s="44"/>
       <c r="I37" s="44"/>
     </row>
-    <row r="38" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="42" t="s">
         <v>143</v>
       </c>

</xml_diff>